<commit_message>
Speed up of 2.4
</commit_message>
<xml_diff>
--- a/Report/SpeedUp.xlsx
+++ b/Report/SpeedUp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhanukagamage/Dropbox/Monash University/FIT3143/Assignment 2/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162E3ADC-B855-3642-AD6E-7AFBECD78815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEBBD8-E758-E246-A825-3C8C37449DAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="4740" windowWidth="28800" windowHeight="33820" activeTab="4" xr2:uid="{F3CA6A85-1115-7645-940B-AB59F541C353}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="19180" activeTab="2" xr2:uid="{F3CA6A85-1115-7645-940B-AB59F541C353}"/>
   </bookViews>
   <sheets>
     <sheet name="tt" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>Iteration</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Dyan</t>
+  </si>
+  <si>
+    <t>Dynamic</t>
   </si>
 </sst>
 </file>
@@ -11144,10 +11147,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761CBA4C-D172-AC47-AA23-C429FA586896}">
-  <dimension ref="D2:Q259"/>
+  <dimension ref="A2:Q259"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67:J139"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11156,7 +11159,7 @@
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="N2" t="s">
         <v>27</v>
       </c>
@@ -11170,7 +11173,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3.8406000000000003E-2</v>
+      </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
@@ -11199,7 +11213,10 @@
         <v>2.4326E-2</v>
       </c>
     </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3.2792000000000002E-2</v>
+      </c>
       <c r="D6">
         <v>3.2599999999999999E-3</v>
       </c>
@@ -11222,7 +11239,10 @@
         <v>2.3328000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3.4861999999999997E-2</v>
+      </c>
       <c r="D7">
         <v>1.2960000000000001E-3</v>
       </c>
@@ -11245,7 +11265,10 @@
         <v>4.2486000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3.5360000000000003E-2</v>
+      </c>
       <c r="D8">
         <v>1.9100000000000001E-4</v>
       </c>
@@ -11268,7 +11291,10 @@
         <v>2.7385E-2</v>
       </c>
     </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3.7095999999999997E-2</v>
+      </c>
       <c r="D9">
         <v>7.2900000000000005E-4</v>
       </c>
@@ -11291,7 +11317,10 @@
         <v>7.5443999999999997E-2</v>
       </c>
     </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5.6238000000000003E-2</v>
+      </c>
       <c r="D10">
         <v>5.4029999999999998E-3</v>
       </c>
@@ -11314,7 +11343,10 @@
         <v>4.8530999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5.6250000000000001E-2</v>
+      </c>
       <c r="D11">
         <v>5.2129999999999998E-3</v>
       </c>
@@ -11337,7 +11369,10 @@
         <v>4.8611000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5.7583000000000002E-2</v>
+      </c>
       <c r="D12">
         <v>5.5589999999999997E-3</v>
       </c>
@@ -11360,7 +11395,10 @@
         <v>2.9513000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5.6698999999999999E-2</v>
+      </c>
       <c r="D13">
         <v>5.489E-3</v>
       </c>
@@ -11383,7 +11421,10 @@
         <v>0.14466799999999999</v>
       </c>
     </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3.8774000000000003E-2</v>
+      </c>
       <c r="D14">
         <v>5.7910000000000001E-3</v>
       </c>
@@ -11406,7 +11447,10 @@
         <v>8.5402000000000006E-2</v>
       </c>
     </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3.789E-2</v>
+      </c>
       <c r="D15">
         <v>7.4700000000000005E-4</v>
       </c>
@@ -11429,7 +11473,10 @@
         <v>3.7969000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3.7024000000000001E-2</v>
+      </c>
       <c r="D16">
         <v>1.4319999999999999E-3</v>
       </c>
@@ -11452,7 +11499,10 @@
         <v>6.2911999999999996E-2</v>
       </c>
     </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3.2849999999999997E-2</v>
+      </c>
       <c r="D17">
         <v>1.9710000000000001E-3</v>
       </c>
@@ -11475,7 +11525,10 @@
         <v>4.8287999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3.4405999999999999E-2</v>
+      </c>
       <c r="D18">
         <v>2.2309999999999999E-3</v>
       </c>
@@ -11498,7 +11551,10 @@
         <v>5.6764000000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>5.6388000000000001E-2</v>
+      </c>
       <c r="D19">
         <v>1.596E-3</v>
       </c>
@@ -11521,7 +11577,10 @@
         <v>0.183757</v>
       </c>
     </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5.6957000000000001E-2</v>
+      </c>
       <c r="D20">
         <v>4.8299999999999998E-4</v>
       </c>
@@ -11544,7 +11603,10 @@
         <v>6.2644000000000005E-2</v>
       </c>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>5.7287999999999999E-2</v>
+      </c>
       <c r="D21">
         <v>7.7899999999999996E-4</v>
       </c>
@@ -11567,7 +11629,10 @@
         <v>4.0001000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3.8351999999999997E-2</v>
+      </c>
       <c r="D22">
         <v>2.0660000000000001E-3</v>
       </c>
@@ -11590,7 +11655,10 @@
         <v>4.4734999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3.6831000000000003E-2</v>
+      </c>
       <c r="D23">
         <v>2.297E-3</v>
       </c>
@@ -11613,7 +11681,10 @@
         <v>3.8958E-2</v>
       </c>
     </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3.5052E-2</v>
+      </c>
       <c r="D24">
         <v>2.3E-3</v>
       </c>
@@ -11636,7 +11707,10 @@
         <v>4.9216999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3.5587000000000001E-2</v>
+      </c>
       <c r="D25">
         <v>2.0349999999999999E-3</v>
       </c>
@@ -11659,7 +11733,10 @@
         <v>0.15012300000000001</v>
       </c>
     </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3.4651000000000001E-2</v>
+      </c>
       <c r="D26">
         <v>5.2400000000000005E-4</v>
       </c>
@@ -11682,7 +11759,10 @@
         <v>0.23197400000000001</v>
       </c>
     </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5.7242000000000001E-2</v>
+      </c>
       <c r="D27">
         <v>7.7099999999999998E-4</v>
       </c>
@@ -11705,7 +11785,10 @@
         <v>9.1670000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5.6651E-2</v>
+      </c>
       <c r="D28">
         <v>9.9599999999999992E-4</v>
       </c>
@@ -11728,7 +11811,10 @@
         <v>9.5481999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>5.9811999999999997E-2</v>
+      </c>
       <c r="D29">
         <v>8.2399999999999997E-4</v>
       </c>
@@ -11751,7 +11837,10 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5.6482999999999998E-2</v>
+      </c>
       <c r="D30">
         <v>6.8400000000000004E-4</v>
       </c>
@@ -11774,7 +11863,10 @@
         <v>2.7474999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4.0740999999999999E-2</v>
+      </c>
       <c r="D31">
         <v>5.62E-4</v>
       </c>
@@ -11797,7 +11889,10 @@
         <v>0.11612</v>
       </c>
     </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3.6032000000000002E-2</v>
+      </c>
       <c r="D32">
         <v>7.5299999999999998E-4</v>
       </c>
@@ -11820,7 +11915,10 @@
         <v>0.101627</v>
       </c>
     </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3.6524000000000001E-2</v>
+      </c>
       <c r="D33">
         <v>5.7559999999999998E-3</v>
       </c>
@@ -11843,7 +11941,10 @@
         <v>5.0458000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3.6176E-2</v>
+      </c>
       <c r="D34">
         <v>5.9680000000000002E-3</v>
       </c>
@@ -11866,7 +11967,10 @@
         <v>3.8975000000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3.5614E-2</v>
+      </c>
       <c r="D35">
         <v>6.2989999999999999E-3</v>
       </c>
@@ -11889,7 +11993,10 @@
         <v>9.7587999999999994E-2</v>
       </c>
     </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5.5400999999999999E-2</v>
+      </c>
       <c r="D36">
         <v>5.8719999999999996E-3</v>
       </c>
@@ -11912,7 +12019,10 @@
         <v>5.8737999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3.7169000000000001E-2</v>
+      </c>
       <c r="D37">
         <v>6.1720000000000004E-3</v>
       </c>
@@ -11935,7 +12045,10 @@
         <v>8.4185999999999997E-2</v>
       </c>
     </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3.4518E-2</v>
+      </c>
       <c r="D38">
         <v>1.6100000000000001E-4</v>
       </c>
@@ -11958,7 +12071,10 @@
         <v>0.100733</v>
       </c>
     </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3.5251999999999999E-2</v>
+      </c>
       <c r="D39">
         <v>1.9799999999999999E-4</v>
       </c>
@@ -11981,7 +12097,10 @@
         <v>7.1958999999999995E-2</v>
       </c>
     </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3.6902999999999998E-2</v>
+      </c>
       <c r="D40">
         <v>1.01E-4</v>
       </c>
@@ -12004,7 +12123,10 @@
         <v>3.3683999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3.4741000000000001E-2</v>
+      </c>
       <c r="D41">
         <v>3.1E-4</v>
       </c>
@@ -12027,7 +12149,10 @@
         <v>0.23037099999999999</v>
       </c>
     </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5.7209999999999997E-2</v>
+      </c>
       <c r="D42">
         <v>8.5099999999999998E-4</v>
       </c>
@@ -12050,7 +12175,10 @@
         <v>0.128859</v>
       </c>
     </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5.7362999999999997E-2</v>
+      </c>
       <c r="D43">
         <v>4.8899999999999996E-4</v>
       </c>
@@ -12073,7 +12201,10 @@
         <v>0.18535199999999999</v>
       </c>
     </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>5.7259999999999998E-2</v>
+      </c>
       <c r="D44">
         <v>4.8520000000000004E-3</v>
       </c>
@@ -12093,7 +12224,10 @@
         <v>0.136488</v>
       </c>
     </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5.5191999999999998E-2</v>
+      </c>
       <c r="D45">
         <v>5.2830000000000004E-3</v>
       </c>
@@ -12113,7 +12247,10 @@
         <v>5.8845000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3.7017000000000001E-2</v>
+      </c>
       <c r="D46">
         <v>5.3899999999999998E-3</v>
       </c>
@@ -12133,7 +12270,10 @@
         <v>5.4468999999999997E-2</v>
       </c>
     </row>
-    <row r="47" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>3.8017000000000002E-2</v>
+      </c>
       <c r="D47">
         <v>1.1039999999999999E-3</v>
       </c>
@@ -12150,7 +12290,10 @@
         <v>7.5442999999999996E-2</v>
       </c>
     </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3.7067000000000003E-2</v>
+      </c>
       <c r="D48">
         <v>6.8599999999999998E-4</v>
       </c>
@@ -12167,7 +12310,10 @@
         <v>6.2049E-2</v>
       </c>
     </row>
-    <row r="49" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3.6074000000000002E-2</v>
+      </c>
       <c r="D49">
         <v>5.4190000000000002E-3</v>
       </c>
@@ -12184,7 +12330,10 @@
         <v>0.33216099999999998</v>
       </c>
     </row>
-    <row r="50" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>4.0309999999999999E-2</v>
+      </c>
       <c r="D50">
         <v>5.7629999999999999E-3</v>
       </c>
@@ -12209,7 +12358,10 @@
         <v>0.13633999999999999</v>
       </c>
     </row>
-    <row r="51" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5.7855999999999998E-2</v>
+      </c>
       <c r="D51">
         <v>6.0679999999999996E-3</v>
       </c>
@@ -12226,7 +12378,10 @@
         <v>0.14674599999999999</v>
       </c>
     </row>
-    <row r="52" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>5.6701000000000001E-2</v>
+      </c>
       <c r="D52">
         <v>6.5929999999999999E-3</v>
       </c>
@@ -12243,7 +12398,10 @@
         <v>0.326067</v>
       </c>
     </row>
-    <row r="53" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>4.1480000000000003E-2</v>
+      </c>
       <c r="D53">
         <v>6.4799999999999996E-3</v>
       </c>
@@ -12260,7 +12418,10 @@
         <v>0.32636700000000002</v>
       </c>
     </row>
-    <row r="54" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>3.5374999999999997E-2</v>
+      </c>
       <c r="D54">
         <v>5.973E-3</v>
       </c>
@@ -12277,7 +12438,10 @@
         <v>0.17612900000000001</v>
       </c>
     </row>
-    <row r="55" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>3.6019000000000002E-2</v>
+      </c>
       <c r="D55">
         <v>6.3889999999999997E-3</v>
       </c>
@@ -12299,7 +12463,10 @@
         <v>0.37885000000000002</v>
       </c>
     </row>
-    <row r="56" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>3.6276000000000003E-2</v>
+      </c>
       <c r="D56">
         <v>6.509E-3</v>
       </c>
@@ -12313,7 +12480,10 @@
         <v>0.157332</v>
       </c>
     </row>
-    <row r="57" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>3.5840999999999998E-2</v>
+      </c>
       <c r="N57">
         <v>0.90463800000000005</v>
       </c>
@@ -12324,7 +12494,10 @@
         <v>8.7899000000000005E-2</v>
       </c>
     </row>
-    <row r="58" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>0.107765</v>
+      </c>
       <c r="D58">
         <f>AVERAGE(D6:D56)</f>
         <v>3.0327058823529413E-3</v>
@@ -12336,52 +12509,61 @@
         <v>6.4811999999999995E-2</v>
       </c>
     </row>
-    <row r="59" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3.9233999999999998E-2</v>
+      </c>
       <c r="N59" s="11"/>
       <c r="P59">
         <v>6.3898999999999997E-2</v>
       </c>
     </row>
-    <row r="60" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>4.1216000000000003E-2</v>
+      </c>
       <c r="N60" s="11"/>
       <c r="P60">
         <v>0.46150600000000003</v>
       </c>
     </row>
-    <row r="61" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>4.3656E-2</v>
+      </c>
       <c r="N61" s="11"/>
       <c r="P61">
         <v>0.33319199999999999</v>
       </c>
     </row>
-    <row r="62" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="N62" s="11"/>
       <c r="P62">
         <v>0.195109</v>
       </c>
     </row>
-    <row r="63" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="N63" s="11"/>
       <c r="P63">
         <v>0.22553400000000001</v>
       </c>
     </row>
-    <row r="64" spans="4:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="N64" s="11"/>
     </row>
-    <row r="65" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N65" s="11"/>
     </row>
-    <row r="66" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N66" s="11"/>
     </row>
-    <row r="67" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N67" s="11"/>
     </row>
-    <row r="68" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N68" s="11"/>
     </row>
-    <row r="69" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N69" s="11">
         <f>AVERAGE(N5:N58)</f>
         <v>0.26949368518518518</v>
@@ -12399,7 +12581,7 @@
         <v>9.9478340000000026E-2</v>
       </c>
     </row>
-    <row r="70" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E70" t="s">
         <v>27</v>
       </c>
@@ -12411,7 +12593,16 @@
       </c>
       <c r="N70" s="11"/>
     </row>
-    <row r="71" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>2.8858999999999999E-2</v>
+      </c>
+      <c r="C71">
+        <v>2.8840000000000001E-2</v>
+      </c>
+      <c r="D71">
+        <v>2.8844000000000002E-2</v>
+      </c>
       <c r="E71">
         <v>7.0063E-2</v>
       </c>
@@ -12435,7 +12626,16 @@
         <v>2.7090689810986501</v>
       </c>
     </row>
-    <row r="72" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>2.8843000000000001E-2</v>
+      </c>
+      <c r="C72">
+        <v>2.8839E-2</v>
+      </c>
+      <c r="D72">
+        <v>2.8853E-2</v>
+      </c>
       <c r="E72">
         <v>5.0494999999999998E-2</v>
       </c>
@@ -12447,7 +12647,16 @@
       </c>
       <c r="N72" s="11"/>
     </row>
-    <row r="73" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>2.8882999999999999E-2</v>
+      </c>
+      <c r="C73">
+        <v>2.8851999999999999E-2</v>
+      </c>
+      <c r="D73">
+        <v>2.8867E-2</v>
+      </c>
       <c r="E73">
         <v>8.1269999999999995E-2</v>
       </c>
@@ -12459,7 +12668,16 @@
       </c>
       <c r="N73" s="11"/>
     </row>
-    <row r="74" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>2.8867E-2</v>
+      </c>
+      <c r="C74">
+        <v>2.8823999999999999E-2</v>
+      </c>
+      <c r="D74">
+        <v>2.8910000000000002E-2</v>
+      </c>
       <c r="E74">
         <v>6.3300999999999996E-2</v>
       </c>
@@ -12471,7 +12689,16 @@
       </c>
       <c r="N74" s="11"/>
     </row>
-    <row r="75" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>2.8871999999999998E-2</v>
+      </c>
+      <c r="C75">
+        <v>2.8826999999999998E-2</v>
+      </c>
+      <c r="D75">
+        <v>2.8854000000000001E-2</v>
+      </c>
       <c r="E75">
         <v>7.1858000000000005E-2</v>
       </c>
@@ -12483,7 +12710,16 @@
       </c>
       <c r="N75" s="11"/>
     </row>
-    <row r="76" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>2.8858999999999999E-2</v>
+      </c>
+      <c r="C76">
+        <v>2.8837000000000002E-2</v>
+      </c>
+      <c r="D76">
+        <v>2.8851999999999999E-2</v>
+      </c>
       <c r="E76">
         <v>6.4679E-2</v>
       </c>
@@ -12495,7 +12731,16 @@
       </c>
       <c r="N76" s="11"/>
     </row>
-    <row r="77" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>2.8879999999999999E-2</v>
+      </c>
+      <c r="C77">
+        <v>2.8826999999999998E-2</v>
+      </c>
+      <c r="D77">
+        <v>2.8857000000000001E-2</v>
+      </c>
       <c r="E77">
         <v>8.0365000000000006E-2</v>
       </c>
@@ -12507,7 +12752,16 @@
       </c>
       <c r="N77" s="11"/>
     </row>
-    <row r="78" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>2.8843000000000001E-2</v>
+      </c>
+      <c r="C78">
+        <v>2.8833000000000001E-2</v>
+      </c>
+      <c r="D78">
+        <v>2.8899000000000001E-2</v>
+      </c>
       <c r="E78">
         <v>7.9764000000000002E-2</v>
       </c>
@@ -12519,7 +12773,16 @@
       </c>
       <c r="N78" s="11"/>
     </row>
-    <row r="79" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>2.8871000000000001E-2</v>
+      </c>
+      <c r="C79">
+        <v>2.8833000000000001E-2</v>
+      </c>
+      <c r="D79">
+        <v>2.8868999999999999E-2</v>
+      </c>
       <c r="E79">
         <v>8.3387000000000003E-2</v>
       </c>
@@ -12531,7 +12794,16 @@
       </c>
       <c r="N79" s="11"/>
     </row>
-    <row r="80" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>2.8857000000000001E-2</v>
+      </c>
+      <c r="C80">
+        <v>2.8825E-2</v>
+      </c>
+      <c r="D80">
+        <v>2.8916000000000001E-2</v>
+      </c>
       <c r="E80">
         <v>7.3814000000000005E-2</v>
       </c>
@@ -12543,7 +12815,16 @@
       </c>
       <c r="N80" s="11"/>
     </row>
-    <row r="81" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>2.8872999999999999E-2</v>
+      </c>
+      <c r="C81">
+        <v>2.8840999999999999E-2</v>
+      </c>
+      <c r="D81">
+        <v>2.8895000000000001E-2</v>
+      </c>
       <c r="E81">
         <v>7.4125999999999997E-2</v>
       </c>
@@ -12555,7 +12836,16 @@
       </c>
       <c r="N81" s="11"/>
     </row>
-    <row r="82" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>2.8856E-2</v>
+      </c>
+      <c r="C82">
+        <v>2.8822E-2</v>
+      </c>
+      <c r="D82">
+        <v>2.8919E-2</v>
+      </c>
       <c r="E82">
         <v>8.6222999999999994E-2</v>
       </c>
@@ -12567,7 +12857,16 @@
       </c>
       <c r="N82" s="11"/>
     </row>
-    <row r="83" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>2.8857000000000001E-2</v>
+      </c>
+      <c r="C83">
+        <v>2.8844000000000002E-2</v>
+      </c>
+      <c r="D83">
+        <v>2.8844000000000002E-2</v>
+      </c>
       <c r="E83">
         <v>7.9836000000000004E-2</v>
       </c>
@@ -12579,7 +12878,16 @@
       </c>
       <c r="N83" s="11"/>
     </row>
-    <row r="84" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>2.8863E-2</v>
+      </c>
+      <c r="C84">
+        <v>2.8837999999999999E-2</v>
+      </c>
+      <c r="D84">
+        <v>2.8837000000000002E-2</v>
+      </c>
       <c r="E84">
         <v>9.0804999999999997E-2</v>
       </c>
@@ -12591,7 +12899,16 @@
       </c>
       <c r="N84" s="11"/>
     </row>
-    <row r="85" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>2.8858000000000002E-2</v>
+      </c>
+      <c r="C85">
+        <v>2.8812000000000001E-2</v>
+      </c>
+      <c r="D85">
+        <v>2.8875000000000001E-2</v>
+      </c>
       <c r="E85">
         <v>7.8768000000000005E-2</v>
       </c>
@@ -12603,7 +12920,16 @@
       </c>
       <c r="N85" s="11"/>
     </row>
-    <row r="86" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>2.8856E-2</v>
+      </c>
+      <c r="C86">
+        <v>2.8819999999999998E-2</v>
+      </c>
+      <c r="D86">
+        <v>2.8851999999999999E-2</v>
+      </c>
       <c r="E86">
         <v>8.0002000000000004E-2</v>
       </c>
@@ -12615,7 +12941,16 @@
       </c>
       <c r="N86" s="11"/>
     </row>
-    <row r="87" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>2.8867E-2</v>
+      </c>
+      <c r="C87">
+        <v>2.8833999999999999E-2</v>
+      </c>
+      <c r="D87">
+        <v>2.8832E-2</v>
+      </c>
       <c r="E87">
         <v>6.6696000000000005E-2</v>
       </c>
@@ -12627,7 +12962,16 @@
       </c>
       <c r="N87" s="11"/>
     </row>
-    <row r="88" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>2.8874E-2</v>
+      </c>
+      <c r="C88">
+        <v>2.8840000000000001E-2</v>
+      </c>
+      <c r="D88">
+        <v>2.8842E-2</v>
+      </c>
       <c r="E88">
         <v>6.1275000000000003E-2</v>
       </c>
@@ -12639,7 +12983,16 @@
       </c>
       <c r="N88" s="11"/>
     </row>
-    <row r="89" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>2.8864999999999998E-2</v>
+      </c>
+      <c r="C89">
+        <v>2.8833000000000001E-2</v>
+      </c>
+      <c r="D89">
+        <v>2.8829E-2</v>
+      </c>
       <c r="E89">
         <v>7.4587000000000001E-2</v>
       </c>
@@ -12651,7 +13004,16 @@
       </c>
       <c r="N89" s="11"/>
     </row>
-    <row r="90" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>2.8886999999999999E-2</v>
+      </c>
+      <c r="C90">
+        <v>2.8820999999999999E-2</v>
+      </c>
+      <c r="D90">
+        <v>2.8868000000000001E-2</v>
+      </c>
       <c r="E90">
         <v>7.2135000000000005E-2</v>
       </c>
@@ -12663,7 +13025,16 @@
       </c>
       <c r="N90" s="11"/>
     </row>
-    <row r="91" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>2.8892000000000001E-2</v>
+      </c>
+      <c r="C91">
+        <v>2.8833999999999999E-2</v>
+      </c>
+      <c r="D91">
+        <v>2.8854000000000001E-2</v>
+      </c>
       <c r="E91">
         <v>8.0325999999999995E-2</v>
       </c>
@@ -12675,7 +13046,16 @@
       </c>
       <c r="N91" s="11"/>
     </row>
-    <row r="92" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>2.8854999999999999E-2</v>
+      </c>
+      <c r="C92">
+        <v>2.8843000000000001E-2</v>
+      </c>
+      <c r="D92">
+        <v>2.8878000000000001E-2</v>
+      </c>
       <c r="E92">
         <v>8.2818000000000003E-2</v>
       </c>
@@ -12687,7 +13067,16 @@
       </c>
       <c r="N92" s="11"/>
     </row>
-    <row r="93" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>2.8850000000000001E-2</v>
+      </c>
+      <c r="C93">
+        <v>2.8823000000000001E-2</v>
+      </c>
+      <c r="D93">
+        <v>2.8858000000000002E-2</v>
+      </c>
       <c r="E93">
         <v>0.10129199999999999</v>
       </c>
@@ -12699,7 +13088,16 @@
       </c>
       <c r="N93" s="11"/>
     </row>
-    <row r="94" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>2.8878999999999998E-2</v>
+      </c>
+      <c r="C94">
+        <v>2.8861999999999999E-2</v>
+      </c>
+      <c r="D94">
+        <v>2.8847999999999999E-2</v>
+      </c>
       <c r="E94">
         <v>6.8283999999999997E-2</v>
       </c>
@@ -12711,7 +13109,16 @@
       </c>
       <c r="N94" s="11"/>
     </row>
-    <row r="95" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>2.8850000000000001E-2</v>
+      </c>
+      <c r="C95">
+        <v>2.8816000000000001E-2</v>
+      </c>
+      <c r="D95">
+        <v>2.8839E-2</v>
+      </c>
       <c r="E95">
         <v>7.6713000000000003E-2</v>
       </c>
@@ -12723,7 +13130,16 @@
       </c>
       <c r="N95" s="11"/>
     </row>
-    <row r="96" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>2.8919E-2</v>
+      </c>
+      <c r="C96">
+        <v>2.8840999999999999E-2</v>
+      </c>
+      <c r="D96">
+        <v>2.8851000000000002E-2</v>
+      </c>
       <c r="E96">
         <v>7.5924000000000005E-2</v>
       </c>
@@ -12735,7 +13151,16 @@
       </c>
       <c r="N96" s="11"/>
     </row>
-    <row r="97" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>2.8910000000000002E-2</v>
+      </c>
+      <c r="C97">
+        <v>2.8839E-2</v>
+      </c>
+      <c r="D97">
+        <v>2.8836000000000001E-2</v>
+      </c>
       <c r="E97">
         <v>0.102969</v>
       </c>
@@ -12747,7 +13172,16 @@
       </c>
       <c r="N97" s="11"/>
     </row>
-    <row r="98" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>2.8910000000000002E-2</v>
+      </c>
+      <c r="C98">
+        <v>2.8842E-2</v>
+      </c>
+      <c r="D98">
+        <v>2.8830000000000001E-2</v>
+      </c>
       <c r="E98">
         <v>8.0950999999999995E-2</v>
       </c>
@@ -12759,7 +13193,16 @@
       </c>
       <c r="N98" s="11"/>
     </row>
-    <row r="99" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>2.8896999999999999E-2</v>
+      </c>
+      <c r="C99">
+        <v>2.8826999999999998E-2</v>
+      </c>
+      <c r="D99">
+        <v>2.9475000000000001E-2</v>
+      </c>
       <c r="E99">
         <v>7.0602999999999999E-2</v>
       </c>
@@ -12771,7 +13214,16 @@
       </c>
       <c r="N99" s="11"/>
     </row>
-    <row r="100" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>2.8898E-2</v>
+      </c>
+      <c r="C100">
+        <v>2.8840999999999999E-2</v>
+      </c>
+      <c r="D100">
+        <v>2.8836000000000001E-2</v>
+      </c>
       <c r="E100">
         <v>7.0326E-2</v>
       </c>
@@ -12783,7 +13235,16 @@
       </c>
       <c r="N100" s="11"/>
     </row>
-    <row r="101" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>2.8885000000000001E-2</v>
+      </c>
+      <c r="C101">
+        <v>2.8837000000000002E-2</v>
+      </c>
+      <c r="D101">
+        <v>2.8822E-2</v>
+      </c>
       <c r="E101">
         <v>7.1831000000000006E-2</v>
       </c>
@@ -12795,7 +13256,16 @@
       </c>
       <c r="N101" s="11"/>
     </row>
-    <row r="102" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>2.8927999999999999E-2</v>
+      </c>
+      <c r="C102">
+        <v>2.8840999999999999E-2</v>
+      </c>
+      <c r="D102">
+        <v>2.8826000000000001E-2</v>
+      </c>
       <c r="E102">
         <v>7.0125999999999994E-2</v>
       </c>
@@ -12807,7 +13277,16 @@
       </c>
       <c r="N102" s="11"/>
     </row>
-    <row r="103" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>2.8889000000000001E-2</v>
+      </c>
+      <c r="C103">
+        <v>2.8826999999999998E-2</v>
+      </c>
+      <c r="D103">
+        <v>2.8827999999999999E-2</v>
+      </c>
       <c r="E103">
         <v>8.3438999999999999E-2</v>
       </c>
@@ -12819,7 +13298,16 @@
       </c>
       <c r="N103" s="11"/>
     </row>
-    <row r="104" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>2.8892999999999999E-2</v>
+      </c>
+      <c r="C104">
+        <v>2.8854999999999999E-2</v>
+      </c>
+      <c r="D104">
+        <v>2.8823000000000001E-2</v>
+      </c>
       <c r="E104">
         <v>6.6424999999999998E-2</v>
       </c>
@@ -12831,7 +13319,16 @@
       </c>
       <c r="N104" s="11"/>
     </row>
-    <row r="105" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>2.8913999999999999E-2</v>
+      </c>
+      <c r="C105">
+        <v>2.8833999999999999E-2</v>
+      </c>
+      <c r="D105">
+        <v>2.8829E-2</v>
+      </c>
       <c r="E105">
         <v>8.2036999999999999E-2</v>
       </c>
@@ -12843,7 +13340,16 @@
       </c>
       <c r="N105" s="11"/>
     </row>
-    <row r="106" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>2.8899000000000001E-2</v>
+      </c>
+      <c r="C106">
+        <v>2.8951999999999999E-2</v>
+      </c>
+      <c r="D106">
+        <v>2.8809999999999999E-2</v>
+      </c>
       <c r="E106">
         <v>0.125695</v>
       </c>
@@ -12855,7 +13361,16 @@
       </c>
       <c r="N106" s="11"/>
     </row>
-    <row r="107" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>2.8889000000000001E-2</v>
+      </c>
+      <c r="C107">
+        <v>2.8854999999999999E-2</v>
+      </c>
+      <c r="D107">
+        <v>2.8819000000000001E-2</v>
+      </c>
       <c r="E107">
         <v>0.14100799999999999</v>
       </c>
@@ -12867,7 +13382,16 @@
       </c>
       <c r="N107" s="11"/>
     </row>
-    <row r="108" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>2.8892999999999999E-2</v>
+      </c>
+      <c r="C108">
+        <v>2.8839E-2</v>
+      </c>
+      <c r="D108">
+        <v>2.8804E-2</v>
+      </c>
       <c r="E108">
         <v>0.125861</v>
       </c>
@@ -12879,7 +13403,16 @@
       </c>
       <c r="N108" s="11"/>
     </row>
-    <row r="109" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>2.8917000000000002E-2</v>
+      </c>
+      <c r="C109">
+        <v>2.8882999999999999E-2</v>
+      </c>
+      <c r="D109">
+        <v>2.9316999999999999E-2</v>
+      </c>
       <c r="E109">
         <v>9.8128000000000007E-2</v>
       </c>
@@ -12891,7 +13424,16 @@
       </c>
       <c r="N109" s="11"/>
     </row>
-    <row r="110" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>2.8881E-2</v>
+      </c>
+      <c r="C110">
+        <v>2.8830999999999999E-2</v>
+      </c>
+      <c r="D110">
+        <v>2.8801E-2</v>
+      </c>
       <c r="E110">
         <v>6.9325999999999999E-2</v>
       </c>
@@ -12903,7 +13445,16 @@
       </c>
       <c r="N110" s="11"/>
     </row>
-    <row r="111" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>2.8892000000000001E-2</v>
+      </c>
+      <c r="C111">
+        <v>2.8809999999999999E-2</v>
+      </c>
+      <c r="D111">
+        <v>2.8844000000000002E-2</v>
+      </c>
       <c r="E111">
         <v>6.8283999999999997E-2</v>
       </c>
@@ -12912,7 +13463,16 @@
       </c>
       <c r="N111" s="11"/>
     </row>
-    <row r="112" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>2.8902000000000001E-2</v>
+      </c>
+      <c r="C112">
+        <v>2.8785999999999999E-2</v>
+      </c>
+      <c r="D112">
+        <v>2.8808E-2</v>
+      </c>
       <c r="E112">
         <v>7.0650000000000004E-2</v>
       </c>
@@ -12921,7 +13481,16 @@
       </c>
       <c r="N112" s="11"/>
     </row>
-    <row r="113" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>2.8910000000000002E-2</v>
+      </c>
+      <c r="C113">
+        <v>2.8812999999999998E-2</v>
+      </c>
+      <c r="D113">
+        <v>2.8830999999999999E-2</v>
+      </c>
       <c r="E113">
         <v>0.15545800000000001</v>
       </c>
@@ -12934,7 +13503,16 @@
       </c>
       <c r="N113" s="11"/>
     </row>
-    <row r="114" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>2.8895000000000001E-2</v>
+      </c>
+      <c r="C114">
+        <v>2.8816000000000001E-2</v>
+      </c>
+      <c r="D114">
+        <v>2.8815E-2</v>
+      </c>
       <c r="E114">
         <v>0.116858</v>
       </c>
@@ -12942,7 +13520,16 @@
         <v>1.3348E-2</v>
       </c>
     </row>
-    <row r="115" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>2.8881E-2</v>
+      </c>
+      <c r="C115">
+        <v>2.8802999999999999E-2</v>
+      </c>
+      <c r="D115">
+        <v>2.8813999999999999E-2</v>
+      </c>
       <c r="E115">
         <v>6.0907000000000003E-2</v>
       </c>
@@ -12951,7 +13538,16 @@
       </c>
       <c r="N115" s="11"/>
     </row>
-    <row r="116" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>2.8915E-2</v>
+      </c>
+      <c r="C116">
+        <v>2.8813999999999999E-2</v>
+      </c>
+      <c r="D116">
+        <v>2.8798000000000001E-2</v>
+      </c>
       <c r="E116">
         <v>6.3353000000000007E-2</v>
       </c>
@@ -12960,7 +13556,16 @@
       </c>
       <c r="N116" s="11"/>
     </row>
-    <row r="117" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>2.8882999999999999E-2</v>
+      </c>
+      <c r="C117">
+        <v>2.8806999999999999E-2</v>
+      </c>
+      <c r="D117">
+        <v>2.8827999999999999E-2</v>
+      </c>
       <c r="E117">
         <v>6.1683000000000002E-2</v>
       </c>
@@ -12969,7 +13574,16 @@
       </c>
       <c r="N117" s="11"/>
     </row>
-    <row r="118" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>2.8854999999999999E-2</v>
+      </c>
+      <c r="C118">
+        <v>2.8826000000000001E-2</v>
+      </c>
+      <c r="D118">
+        <v>2.8816000000000001E-2</v>
+      </c>
       <c r="E118">
         <v>6.3497999999999999E-2</v>
       </c>
@@ -12978,7 +13592,16 @@
       </c>
       <c r="N118" s="11"/>
     </row>
-    <row r="119" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>2.8851999999999999E-2</v>
+      </c>
+      <c r="C119">
+        <v>2.8827999999999999E-2</v>
+      </c>
+      <c r="D119">
+        <v>2.8826000000000001E-2</v>
+      </c>
       <c r="E119">
         <v>6.4878000000000005E-2</v>
       </c>
@@ -12987,82 +13610,208 @@
       </c>
       <c r="N119" s="11"/>
     </row>
-    <row r="120" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>2.887E-2</v>
+      </c>
+      <c r="C120">
+        <v>2.8826000000000001E-2</v>
+      </c>
+      <c r="D120">
+        <v>2.8805000000000001E-2</v>
+      </c>
       <c r="G120">
         <v>1.0067E-2</v>
       </c>
       <c r="N120" s="11"/>
     </row>
-    <row r="121" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>2.8851999999999999E-2</v>
+      </c>
+      <c r="C121">
+        <v>2.8812000000000001E-2</v>
+      </c>
+      <c r="D121">
+        <v>2.8784000000000001E-2</v>
+      </c>
       <c r="G121">
         <v>1.069E-2</v>
       </c>
       <c r="N121" s="11"/>
     </row>
-    <row r="122" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>2.8884E-2</v>
+      </c>
+      <c r="C122">
+        <v>2.8812999999999998E-2</v>
+      </c>
+      <c r="D122">
+        <v>2.8822E-2</v>
+      </c>
       <c r="G122">
         <v>1.4076999999999999E-2</v>
       </c>
       <c r="N122" s="11"/>
     </row>
-    <row r="123" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>2.8853E-2</v>
+      </c>
+      <c r="C123">
+        <v>2.8816999999999999E-2</v>
+      </c>
+      <c r="D123">
+        <v>2.8819000000000001E-2</v>
+      </c>
       <c r="G123">
         <v>4.5488000000000001E-2</v>
       </c>
       <c r="N123" s="11"/>
     </row>
-    <row r="124" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>2.8867E-2</v>
+      </c>
+      <c r="C124">
+        <v>2.8822E-2</v>
+      </c>
+      <c r="D124">
+        <v>2.8802000000000001E-2</v>
+      </c>
       <c r="G124">
         <v>2.495E-2</v>
       </c>
       <c r="N124" s="11"/>
     </row>
-    <row r="125" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>2.896E-2</v>
+      </c>
+      <c r="C125">
+        <v>2.8849E-2</v>
+      </c>
+      <c r="D125">
+        <v>2.8833000000000001E-2</v>
+      </c>
       <c r="G125">
         <v>1.2514000000000001E-2</v>
       </c>
       <c r="N125" s="11"/>
     </row>
-    <row r="126" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>2.9017000000000001E-2</v>
+      </c>
+      <c r="C126">
+        <v>2.8819999999999998E-2</v>
+      </c>
+      <c r="D126">
+        <v>2.8792999999999999E-2</v>
+      </c>
       <c r="G126">
         <v>1.289E-2</v>
       </c>
       <c r="N126" s="11"/>
     </row>
-    <row r="127" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>2.8930000000000001E-2</v>
+      </c>
+      <c r="C127">
+        <v>2.8822E-2</v>
+      </c>
+      <c r="D127">
+        <v>2.8805999999999998E-2</v>
+      </c>
       <c r="G127">
         <v>1.2288E-2</v>
       </c>
       <c r="N127" s="11"/>
     </row>
-    <row r="128" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>2.8884E-2</v>
+      </c>
+      <c r="C128">
+        <v>2.8806999999999999E-2</v>
+      </c>
+      <c r="D128">
+        <v>2.8806999999999999E-2</v>
+      </c>
       <c r="G128">
         <v>1.3632999999999999E-2</v>
       </c>
       <c r="N128" s="11"/>
     </row>
-    <row r="129" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>2.8910999999999999E-2</v>
+      </c>
+      <c r="C129">
+        <v>2.8805000000000001E-2</v>
+      </c>
+      <c r="D129">
+        <v>2.8805000000000001E-2</v>
+      </c>
       <c r="G129">
         <v>1.5396E-2</v>
       </c>
       <c r="N129" s="11"/>
     </row>
-    <row r="130" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>2.8969000000000002E-2</v>
+      </c>
+      <c r="C130">
+        <v>2.8792000000000002E-2</v>
+      </c>
+      <c r="D130">
+        <v>2.8811E-2</v>
+      </c>
       <c r="G130">
         <v>1.2324E-2</v>
       </c>
       <c r="N130" s="11"/>
     </row>
-    <row r="131" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>2.8975000000000001E-2</v>
+      </c>
+      <c r="C131">
+        <v>2.8812000000000001E-2</v>
+      </c>
+      <c r="D131">
+        <v>2.8825E-2</v>
+      </c>
       <c r="N131" s="11"/>
     </row>
-    <row r="132" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C132">
+        <v>2.8802999999999999E-2</v>
+      </c>
+      <c r="D132">
+        <v>2.8819999999999998E-2</v>
+      </c>
       <c r="N132" s="11"/>
     </row>
-    <row r="133" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C133">
+        <v>2.8832E-2</v>
+      </c>
+      <c r="D133">
+        <v>2.8937999999999998E-2</v>
+      </c>
       <c r="N133" s="11"/>
     </row>
-    <row r="134" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C134">
+        <v>2.8833000000000001E-2</v>
+      </c>
+      <c r="D134">
+        <v>2.8805999999999998E-2</v>
+      </c>
       <c r="E134">
         <f>AVERAGE(E71:E119)</f>
         <v>8.0675510204081646E-2</v>
@@ -13073,86 +13822,182 @@
       </c>
       <c r="N134" s="11"/>
     </row>
-    <row r="135" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D135">
+        <v>2.8854000000000001E-2</v>
+      </c>
       <c r="N135" s="11"/>
     </row>
-    <row r="136" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <f>AVERAGE(B71:B131)</f>
+        <v>2.8886803278688519E-2</v>
+      </c>
+      <c r="C136">
+        <f>AVERAGE(C71:C134)</f>
+        <v>2.88301875E-2</v>
+      </c>
+      <c r="D136">
+        <v>2.8809999999999999E-2</v>
+      </c>
       <c r="N136" s="11"/>
     </row>
-    <row r="137" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D137">
+        <v>2.8815E-2</v>
+      </c>
       <c r="N137" s="11"/>
     </row>
-    <row r="138" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D138">
+        <v>2.8795999999999999E-2</v>
+      </c>
+      <c r="E138">
+        <f>D134/G134</f>
+        <v>1.3115734388849092</v>
+      </c>
       <c r="F138">
         <f>E134/G134</f>
         <v>3.6732575280206192</v>
       </c>
       <c r="N138" s="11"/>
     </row>
-    <row r="139" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D139">
+        <v>2.8830000000000001E-2</v>
+      </c>
       <c r="N139" s="11"/>
     </row>
-    <row r="140" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D140">
+        <v>2.8799999999999999E-2</v>
+      </c>
       <c r="N140" s="11"/>
     </row>
-    <row r="141" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <f>D160/B136</f>
+        <v>0.99877866196977838</v>
+      </c>
+      <c r="D141">
+        <v>2.8836000000000001E-2</v>
+      </c>
       <c r="N141" s="11"/>
     </row>
-    <row r="142" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D142">
+        <v>2.8847000000000001E-2</v>
+      </c>
       <c r="N142" s="11"/>
     </row>
-    <row r="143" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D143">
+        <v>2.8816000000000001E-2</v>
+      </c>
       <c r="N143" s="11"/>
     </row>
-    <row r="144" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D144">
+        <v>2.8812999999999998E-2</v>
+      </c>
       <c r="N144" s="11"/>
     </row>
-    <row r="145" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D145">
+        <v>2.8815E-2</v>
+      </c>
       <c r="N145" s="11"/>
     </row>
-    <row r="146" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D146">
+        <v>2.8794E-2</v>
+      </c>
       <c r="N146" s="11"/>
     </row>
-    <row r="147" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D147">
+        <v>2.8809999999999999E-2</v>
+      </c>
       <c r="N147" s="11"/>
     </row>
-    <row r="148" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D148">
+        <v>2.8798000000000001E-2</v>
+      </c>
       <c r="N148" s="11"/>
     </row>
-    <row r="149" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D149">
+        <v>2.8837999999999999E-2</v>
+      </c>
       <c r="N149" s="11"/>
     </row>
-    <row r="150" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C150">
+        <f>D160/C136</f>
+        <v>1.0007400308191796</v>
+      </c>
+      <c r="D150">
+        <v>2.8811E-2</v>
+      </c>
       <c r="N150" s="11"/>
     </row>
-    <row r="151" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D151">
+        <v>2.8924999999999999E-2</v>
+      </c>
       <c r="N151" s="11"/>
     </row>
-    <row r="152" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D152">
+        <v>2.9007000000000002E-2</v>
+      </c>
       <c r="N152" s="11"/>
     </row>
-    <row r="153" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D153">
+        <v>2.8819000000000001E-2</v>
+      </c>
       <c r="N153" s="11"/>
     </row>
-    <row r="154" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D154">
+        <v>2.8850000000000001E-2</v>
+      </c>
       <c r="N154" s="11"/>
     </row>
-    <row r="155" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D155">
+        <v>2.8815E-2</v>
+      </c>
       <c r="N155" s="11"/>
     </row>
-    <row r="156" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D156">
+        <v>2.8851999999999999E-2</v>
+      </c>
       <c r="N156" s="11"/>
     </row>
-    <row r="157" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D157">
+        <v>2.8853E-2</v>
+      </c>
       <c r="N157" s="11"/>
     </row>
-    <row r="158" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D158">
+        <v>2.8975999999999998E-2</v>
+      </c>
       <c r="N158" s="11"/>
     </row>
-    <row r="159" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:14" x14ac:dyDescent="0.2">
       <c r="N159" s="11"/>
     </row>
-    <row r="160" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D160">
+        <f>AVERAGE(D71:D158)</f>
+        <v>2.8851522727272726E-2</v>
+      </c>
       <c r="N160" s="11"/>
     </row>
     <row r="161" spans="14:14" x14ac:dyDescent="0.2">
@@ -29067,8 +29912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722F6530-5160-5D44-BC47-5D8231C5191B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update to final version of the assignment
</commit_message>
<xml_diff>
--- a/Report/SpeedUp.xlsx
+++ b/Report/SpeedUp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhanukagamage/Dropbox/Monash University/FIT3143/Assignment 2/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1427E03D-F687-6B4D-BFC2-B6D6C3266D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1758A06-E0CB-FF4A-A8F0-3E346FAE45A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{F3CA6A85-1115-7645-940B-AB59F541C353}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26980" xr2:uid="{F3CA6A85-1115-7645-940B-AB59F541C353}"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm Analysis" sheetId="3" r:id="rId1"/>
@@ -116,7 +116,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -240,19 +240,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -270,22 +267,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -365,7 +365,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="accent1"/>
                     </a:solidFill>
@@ -980,7 +980,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1445,20 +1445,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3078,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8124BA4-CB04-A242-92BF-3436BBD80A43}">
   <dimension ref="A1:L178"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F26" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="AZ44" sqref="AZ44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3090,22 +3076,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -5517,7 +5503,7 @@
         <v>0.179504</v>
       </c>
       <c r="L69">
-        <f t="shared" ref="L69:L103" si="1">K69/G69</f>
+        <f t="shared" ref="L69:L102" si="1">K69/G69</f>
         <v>4.4875999999999999E-2</v>
       </c>
     </row>
@@ -8040,511 +8026,511 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
     </row>
     <row r="5" spans="1:18" ht="4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I5" s="25"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="25"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
     </row>
     <row r="7" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>112</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>105</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>177</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>2.8102848214285714E-2</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>3.0489800000000015E-2</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>2.9907073446327693E-2</v>
       </c>
-      <c r="I8" s="25"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13">
         <f>C8/D8</f>
         <v>0.92171310452301103</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f>C8/E8</f>
         <v>0.93967229072814806</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>2.5244017857142854E-2</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <v>1.5428999999999995E-2</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>1.3659333333333338E-2</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13">
         <f>C10/D10</f>
         <v>1.6361408942344198</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f>C10/E10</f>
         <v>1.8481149292651797</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
     </row>
     <row r="12" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <f>C8+C10</f>
         <v>5.3346866071428564E-2</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f>D8+D10</f>
         <v>4.591880000000001E-2</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <f>E8+E10</f>
         <v>4.3566406779661032E-2</v>
       </c>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14">
         <f>C12/D12</f>
         <v>1.161765248034107</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <f>C12/E12</f>
         <v>1.2244954315657159</v>
       </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="I17" s="25"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="I18" s="25"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="I19" s="25"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="8"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="I20" s="25"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="8"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8574,39 +8560,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="10" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="F4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="2:8" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -8615,7 +8601,7 @@
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">

</xml_diff>